<commit_message>
Updated BOM to include shorting jumper
</commit_message>
<xml_diff>
--- a/hardware_design/Betweener BOM.xlsx
+++ b/hardware_design/Betweener BOM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="71">
   <si>
     <t>Notes</t>
   </si>
@@ -172,6 +172,9 @@
     <t>512-LM78L05ACZ</t>
   </si>
   <si>
+    <t>shorting jumper</t>
+  </si>
+  <si>
     <t>Optional</t>
   </si>
   <si>
@@ -185,6 +188,9 @@
   </si>
   <si>
     <t>5-pin right-angle male header</t>
+  </si>
+  <si>
+    <t>rainbow ribbon cable?</t>
   </si>
   <si>
     <t>10mm M3 male-female standoff</t>
@@ -224,7 +230,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -258,6 +264,10 @@
       <name val="Arial"/>
     </font>
     <font>
+      <sz val="10.0"/>
+      <color rgb="FF000000"/>
+    </font>
+    <font>
       <u/>
     </font>
   </fonts>
@@ -275,7 +285,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -313,7 +323,14 @@
     <xf borderId="0" fillId="0" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="9" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -412,7 +429,7 @@
         <v>0.012</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F23" si="1">PRODUCT(D3:E3)</f>
+        <f t="shared" ref="F3:F24" si="1">PRODUCT(D3:E3)</f>
         <v>0.048</v>
       </c>
       <c r="H3" s="4" t="str">
@@ -795,181 +812,207 @@
       </c>
     </row>
     <row r="24">
-      <c r="C24" s="10"/>
-      <c r="D24" s="11"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="11"/>
+      <c r="C24" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D24" s="14">
+        <v>1.0</v>
+      </c>
+      <c r="E24" s="14">
+        <v>0.11</v>
+      </c>
+      <c r="F24" s="15">
+        <f t="shared" si="1"/>
+        <v>0.11</v>
+      </c>
       <c r="G24" s="12"/>
       <c r="H24" s="10"/>
+      <c r="I24" s="4" t="str">
+        <f>HYPERLINK("https://www.digikey.com/product-detail/en/sullins-connector-solutions/NPC02SXON-RC/S9341-ND/2618266","S9341-ND")</f>
+        <v>S9341-ND</v>
+      </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="10"/>
+      <c r="D25" s="11"/>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11"/>
+      <c r="G25" s="12"/>
+      <c r="H25" s="10"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="E25" s="1">
+      <c r="C26" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="D26" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="E26" s="1">
         <v>1.35</v>
       </c>
-      <c r="F25">
-        <f>PRODUCT(D25:E25)</f>
+      <c r="F26">
+        <f>PRODUCT(D26:E26)</f>
         <v>1.35</v>
       </c>
-      <c r="H25" s="4" t="str">
+      <c r="H26" s="4" t="str">
         <f>HYPERLINK("https://www.mouser.com/ProductDetail/Adafruit/1833?qs=%2fha2pyFaduh%252bvNW0N9ck%252bdVbqqQ5xYs1pT8%252brArc5drA17FZI6VqEnaF4sUn8S7Yb2CZ1l2Uoio%3d","485-1833")</f>
         <v>485-1833</v>
       </c>
-      <c r="L25" s="5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" s="1" t="s">
+      <c r="L26" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="C26" s="1" t="s">
+    </row>
+    <row r="27">
+      <c r="A27" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="D26" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="I26" s="4" t="str">
+      <c r="C27" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D27" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="I27" s="4" t="str">
         <f>HYPERLINK("https://www.digikey.com/products/en/connectors-interconnects/rectangular-connectors-headers-male-pins/314?k=&amp;pkeyword=&amp;pv88=24&amp;FV=ffe0013a%2Cffec9e0f%2Cfffc0261%2C140716%2C1c0003%2C700002%2Cfc0095%2C1080250%2C114016f%2C1680001%2C16c026f%2C3f00006%2C654001"&amp;"2%2C8000010%2C818000f%2C8d00002%2C9340019%2Cae40008%2Ce1c0008%2C10f00003%2C13bc000c%2C1a740003%2C1bf80001%2C1bfc0009%2C1c00000f%2C1c0c0009%2C1c100014%2C1f140000%2C1f6c0003%2C1f700001%2C1f88014f%2C1f940005%2C1f980001%2C1f9c0001%2C1fa00001%2C1fa40053&amp;quanti"&amp;"ty=0&amp;ColumnSort=0&amp;page=1&amp;pageSize=25","609-4304-ND")</f>
         <v>609-4304-ND</v>
       </c>
     </row>
-    <row r="27" ht="18.75" customHeight="1"/>
-    <row r="28" ht="17.25" customHeight="1">
-      <c r="A28" s="3"/>
-      <c r="B28" s="1"/>
+    <row r="28" ht="18.75" customHeight="1">
       <c r="C28" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="D28" s="1">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="29" ht="18.75" customHeight="1"/>
+    <row r="30" ht="17.25" customHeight="1">
+      <c r="A30" s="3"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D30" s="1">
         <v>2.0</v>
       </c>
-      <c r="E28" s="1">
+      <c r="E30" s="1">
         <v>0.54</v>
       </c>
-      <c r="F28">
-        <f t="shared" ref="F28:F29" si="2">PRODUCT(D28:E28)</f>
+      <c r="F30">
+        <f t="shared" ref="F30:F31" si="2">PRODUCT(D30:E30)</f>
         <v>1.08</v>
       </c>
-      <c r="H28" s="4" t="str">
+      <c r="H30" s="4" t="str">
         <f>HYPERLINK("https://www.mouser.com/ProductDetail/Harwin/R30-3001002?qs=%2fha2pyFadujM3abXvjPvEsRnthYHcP3Cr%252bL%252blzLqeHHEafI7LgZaAw%3d%3d","855-R30-3001002 ")</f>
         <v>855-R30-3001002 </v>
       </c>
-      <c r="M28" s="5" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29">
-      <c r="C29" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="D29" s="1">
+      <c r="M30" s="5" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="C31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D31" s="1">
         <v>5.0</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E31" s="1">
         <v>0.21</v>
       </c>
-      <c r="F29">
+      <c r="F31">
         <f t="shared" si="2"/>
         <v>1.05</v>
       </c>
-      <c r="H29" s="4" t="str">
+      <c r="H31" s="4" t="str">
         <f>HYPERLINK("https://www.mouser.com/ProductDetail/Keystone-Electronics/9191-3?qs=sGAEpiMZZMtFmYSM%2fWUJwujzmQaHftvU5pHcq%2fLayHo%3d","534-9191-3")</f>
         <v>534-9191-3</v>
       </c>
     </row>
-    <row r="30">
-      <c r="A30" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="D30" s="1">
-        <v>1.0</v>
-      </c>
-    </row>
     <row r="32">
-      <c r="A32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="L32" s="1"/>
-    </row>
-    <row r="33">
-      <c r="C33" s="1" t="s">
+      <c r="A32" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="F33">
-        <f>SUM(F3:F32)</f>
-        <v>55.556</v>
+      <c r="C32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="1">
+        <v>1.0</v>
       </c>
     </row>
     <row r="34">
-      <c r="C34" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="F34">
-        <f>F33</f>
-        <v>55.556</v>
+      <c r="A34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="L34" s="1"/>
+    </row>
+    <row r="35">
+      <c r="C35" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F35">
+        <f>SUM(F3:F34)</f>
+        <v>55.666</v>
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="13" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="37">
-      <c r="C37" s="1" t="s">
+      <c r="C36" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="D37" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="E37" s="1">
+      <c r="F36">
+        <f>F35</f>
+        <v>55.666</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" s="16" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="C39" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D39" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="E39" s="1">
         <v>6.5</v>
       </c>
-      <c r="F37" s="1">
-        <f t="shared" ref="F37:F38" si="3">PRODUCT(D37:E37)</f>
+      <c r="F39" s="1">
+        <f t="shared" ref="F39:F40" si="3">PRODUCT(D39:E39)</f>
         <v>6.5</v>
       </c>
-      <c r="J37" s="1"/>
-      <c r="K37" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="C38" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="D38" s="1">
-        <v>1.0</v>
-      </c>
-      <c r="E38" s="1">
+      <c r="J39" s="1"/>
+      <c r="K39" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="C40" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D40" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="E40" s="1">
         <v>6.5</v>
       </c>
-      <c r="F38" s="1">
+      <c r="F40" s="1">
         <f t="shared" si="3"/>
         <v>6.5</v>
       </c>
-      <c r="K38" s="3" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" s="1"/>
+      <c r="K40" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A38:B38"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink r:id="rId1" ref="H4"/>
@@ -989,8 +1032,8 @@
     <hyperlink r:id="rId15" ref="H21"/>
     <hyperlink r:id="rId16" ref="H22"/>
     <hyperlink r:id="rId17" ref="H23"/>
-    <hyperlink r:id="rId18" ref="L25"/>
-    <hyperlink r:id="rId19" location="93655A102" ref="M28"/>
+    <hyperlink r:id="rId18" ref="L26"/>
+    <hyperlink r:id="rId19" location="93655A102" ref="M30"/>
   </hyperlinks>
   <printOptions gridLines="1" horizontalCentered="1"/>
   <pageMargins bottom="0.75" footer="0.0" header="0.0" left="0.7" right="0.7" top="0.75"/>

</xml_diff>